<commit_message>
Add S2 keyword extraction and visualisation
</commit_message>
<xml_diff>
--- a/output/fieldsofstudy_coronavirus.xlsx
+++ b/output/fieldsofstudy_coronavirus.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/610652dada5e09f2/Projects/COVID19_scholcomms/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_FE52BFD56D492CE8EC48BBC631DDED03502DD8D0" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F9881840-8CA0-48E1-993E-5E5D6324B183}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1108,11 +1114,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,6 +1182,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1222,7 +1236,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1254,9 +1268,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1288,6 +1320,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1463,14 +1513,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2909397111</v>
       </c>
@@ -1528,7 +1588,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2910720372</v>
       </c>
@@ -1554,7 +1614,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2909228517</v>
       </c>
@@ -1580,7 +1640,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2908854353</v>
       </c>
@@ -1606,7 +1666,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2908625121</v>
       </c>
@@ -1632,10 +1692,10 @@
         <v>43490</v>
       </c>
       <c r="J6">
-        <v>0.5893436</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>0.58934359999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>142054583</v>
       </c>
@@ -1661,7 +1721,7 @@
         <v>42545</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2781442963</v>
       </c>
@@ -1690,10 +1750,10 @@
         <v>43105</v>
       </c>
       <c r="J8">
-        <v>0.582309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>0.58230899999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2910344980</v>
       </c>
@@ -1719,10 +1779,10 @@
         <v>43490</v>
       </c>
       <c r="J9">
-        <v>0.595625</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>0.59562499999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2775980723</v>
       </c>
@@ -1748,10 +1808,10 @@
         <v>43105</v>
       </c>
       <c r="J10">
-        <v>0.5418491</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>0.54184909999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2911128928</v>
       </c>
@@ -1777,7 +1837,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2910754697</v>
       </c>
@@ -1803,7 +1863,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2911079544</v>
       </c>
@@ -1829,7 +1889,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2778137277</v>
       </c>
@@ -1858,10 +1918,10 @@
         <v>43105</v>
       </c>
       <c r="J14">
-        <v>0.646164954</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>0.64616495399999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2910051538</v>
       </c>
@@ -1887,7 +1947,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2777875948</v>
       </c>
@@ -1916,7 +1976,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16017026</v>
       </c>
@@ -1942,7 +2002,7 @@
         <v>42545</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2776860997</v>
       </c>
@@ -1971,7 +2031,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2909974741</v>
       </c>
@@ -1997,7 +2057,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2779567548</v>
       </c>
@@ -2026,7 +2086,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2781031778</v>
       </c>
@@ -2052,10 +2112,10 @@
         <v>43105</v>
       </c>
       <c r="J21">
-        <v>0.5518072000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>0.55180720000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2908620406</v>
       </c>
@@ -2081,7 +2141,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2778494684</v>
       </c>
@@ -2107,10 +2167,10 @@
         <v>43105</v>
       </c>
       <c r="J23">
-        <v>0.5278989670000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>0.52789896700000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2908738307</v>
       </c>
@@ -2139,7 +2199,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2908654074</v>
       </c>
@@ -2165,7 +2225,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2780987755</v>
       </c>
@@ -2194,10 +2254,10 @@
         <v>43105</v>
       </c>
       <c r="J26">
-        <v>0.604756653</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>0.60475665300000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2908796399</v>
       </c>
@@ -2223,7 +2283,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2908953726</v>
       </c>
@@ -2249,7 +2309,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2908982982</v>
       </c>
@@ -2275,7 +2335,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2780992742</v>
       </c>
@@ -2301,7 +2361,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2780374985</v>
       </c>
@@ -2330,10 +2390,10 @@
         <v>43105</v>
       </c>
       <c r="J31">
-        <v>0.571020067</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>0.57102006699999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2779937474</v>
       </c>
@@ -2359,7 +2419,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2780322730</v>
       </c>
@@ -2388,7 +2448,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2778614427</v>
       </c>
@@ -2414,7 +2474,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2778859668</v>
       </c>
@@ -2443,7 +2503,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2780269264</v>
       </c>
@@ -2469,7 +2529,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2909148942</v>
       </c>
@@ -2495,7 +2555,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2780263450</v>
       </c>
@@ -2521,7 +2581,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2780059724</v>
       </c>
@@ -2547,7 +2607,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2780040827</v>
       </c>
@@ -2576,10 +2636,10 @@
         <v>43105</v>
       </c>
       <c r="J40">
-        <v>0.53954</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>0.53954000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2779973787</v>
       </c>
@@ -2605,10 +2665,10 @@
         <v>43105</v>
       </c>
       <c r="J41">
-        <v>0.5051870000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>0.50518700000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2778860635</v>
       </c>
@@ -2634,7 +2694,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2779954635</v>
       </c>
@@ -2660,7 +2720,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2779944480</v>
       </c>
@@ -2686,7 +2746,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2909005407</v>
       </c>
@@ -2712,7 +2772,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>447327</v>
       </c>
@@ -2738,10 +2798,10 @@
         <v>42545</v>
       </c>
       <c r="J46">
-        <v>0.470971078</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>0.47097107799999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2909175290</v>
       </c>
@@ -2767,7 +2827,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2910932551</v>
       </c>
@@ -2793,7 +2853,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2909893278</v>
       </c>
@@ -2819,7 +2879,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2909895610</v>
       </c>
@@ -2845,7 +2905,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2909931723</v>
       </c>
@@ -2871,7 +2931,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2910187272</v>
       </c>
@@ -2897,7 +2957,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2910187856</v>
       </c>
@@ -2923,7 +2983,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2910188402</v>
       </c>
@@ -2949,7 +3009,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2910257320</v>
       </c>
@@ -2975,7 +3035,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2910332646</v>
       </c>
@@ -3001,7 +3061,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2910412365</v>
       </c>
@@ -3027,7 +3087,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2910515140</v>
       </c>
@@ -3053,7 +3113,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2910600213</v>
       </c>
@@ -3079,7 +3139,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2910736787</v>
       </c>
@@ -3105,7 +3165,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2910793863</v>
       </c>
@@ -3131,7 +3191,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2910910103</v>
       </c>
@@ -3157,7 +3217,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2911094841</v>
       </c>
@@ -3183,7 +3243,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2909228183</v>
       </c>
@@ -3209,7 +3269,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2911165299</v>
       </c>
@@ -3235,7 +3295,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2911177098</v>
       </c>
@@ -3261,7 +3321,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2909756727</v>
       </c>
@@ -3287,7 +3347,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2909608366</v>
       </c>
@@ -3313,7 +3373,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2909598960</v>
       </c>
@@ -3339,7 +3399,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2909587405</v>
       </c>
@@ -3368,7 +3428,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2909528814</v>
       </c>
@@ -3394,7 +3454,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2909513458</v>
       </c>
@@ -3420,7 +3480,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2909509916</v>
       </c>
@@ -3446,7 +3506,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2909460908</v>
       </c>
@@ -3472,7 +3532,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2909433709</v>
       </c>
@@ -3498,7 +3558,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2909433129</v>
       </c>
@@ -3524,7 +3584,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2777675387</v>
       </c>
@@ -3550,7 +3610,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2909376813</v>
       </c>
@@ -3576,7 +3636,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2777691041</v>
       </c>
@@ -3605,10 +3665,10 @@
         <v>43105</v>
       </c>
       <c r="J79">
-        <v>0.6920069</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+        <v>0.69200689999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2778529970</v>
       </c>
@@ -3634,7 +3694,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2909866686</v>
       </c>
@@ -3660,7 +3720,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>58475186</v>
       </c>
@@ -3686,10 +3746,10 @@
         <v>42545</v>
       </c>
       <c r="J82">
-        <v>0.5098353</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+        <v>0.50983529999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>192805744</v>
       </c>
@@ -3715,10 +3775,10 @@
         <v>42545</v>
       </c>
       <c r="J83">
-        <v>0.7211705</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+        <v>0.72117050000000005</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2777485425</v>
       </c>
@@ -3747,10 +3807,10 @@
         <v>43105</v>
       </c>
       <c r="J84">
-        <v>0.6263955</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+        <v>0.62639549999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>187316915</v>
       </c>
@@ -3776,10 +3836,10 @@
         <v>42545</v>
       </c>
       <c r="J85">
-        <v>0.508971632</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+        <v>0.50897163199999995</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2775974701</v>
       </c>
@@ -3805,7 +3865,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>113162765</v>
       </c>
@@ -3831,10 +3891,10 @@
         <v>42545</v>
       </c>
       <c r="J87">
-        <v>0.50101155</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>0.50101154999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2776353676</v>
       </c>
@@ -3866,7 +3926,7 @@
         <v>0.4902416</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2776399701</v>
       </c>
@@ -3895,10 +3955,10 @@
         <v>43105</v>
       </c>
       <c r="J89">
-        <v>0.481211066</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+        <v>0.48121106600000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2776810377</v>
       </c>
@@ -3924,7 +3984,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>76346623</v>
       </c>
@@ -3953,10 +4013,10 @@
         <v>42545</v>
       </c>
       <c r="J91">
-        <v>0.409962535</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+        <v>0.40996253500000002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>67074565</v>
       </c>
@@ -3982,7 +4042,7 @@
         <v>42545</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2776837404</v>
       </c>
@@ -4011,7 +4071,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2776525042</v>
       </c>
@@ -4040,10 +4100,10 @@
         <v>43105</v>
       </c>
       <c r="J94">
-        <v>0.626104534</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+        <v>0.62610453399999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>31567460</v>
       </c>
@@ -4069,7 +4129,7 @@
         <v>42545</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>44048612</v>
       </c>
@@ -4095,10 +4155,10 @@
         <v>42545</v>
       </c>
       <c r="J96">
-        <v>0.4676319</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
+        <v>0.46763189999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>16154277</v>
       </c>
@@ -4124,7 +4184,7 @@
         <v>42545</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2777384484</v>
       </c>
@@ -4153,7 +4213,7 @@
         <v>43105</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>30036603</v>
       </c>
@@ -4179,10 +4239,10 @@
         <v>42545</v>
       </c>
       <c r="J99">
-        <v>0.428689837</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
+        <v>0.42868983700000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>46578552</v>
       </c>
@@ -4208,10 +4268,10 @@
         <v>42545</v>
       </c>
       <c r="J100">
-        <v>0.594227731</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
+        <v>0.59422773100000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>193395930</v>
       </c>
@@ -4240,10 +4300,10 @@
         <v>42545</v>
       </c>
       <c r="J101">
-        <v>0.5796893</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+        <v>0.57968929999999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>44465124</v>
       </c>
@@ -4272,7 +4332,7 @@
         <v>0.4081244</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2776844884</v>
       </c>
@@ -4301,10 +4361,10 @@
         <v>43105</v>
       </c>
       <c r="J103">
-        <v>0.531638861</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+        <v>0.53163886100000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>89138240</v>
       </c>
@@ -4330,10 +4390,10 @@
         <v>42545</v>
       </c>
       <c r="J104">
-        <v>0.52927655</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+        <v>0.52927654999999996</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>89623803</v>
       </c>
@@ -4359,10 +4419,10 @@
         <v>42545</v>
       </c>
       <c r="J105">
-        <v>0.6355718</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
+        <v>0.63557180000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2910753757</v>
       </c>
@@ -4388,10 +4448,10 @@
         <v>43490</v>
       </c>
       <c r="J106">
-        <v>0.438177824</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
+        <v>0.43817782399999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>45189115</v>
       </c>
@@ -4417,10 +4477,10 @@
         <v>42545</v>
       </c>
       <c r="J107">
-        <v>0.447624922</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
+        <v>0.44762492199999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>140704245</v>
       </c>
@@ -4446,10 +4506,10 @@
         <v>42545</v>
       </c>
       <c r="J108">
-        <v>0.469228029</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
+        <v>0.46922802899999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>142052008</v>
       </c>
@@ -4475,10 +4535,10 @@
         <v>42545</v>
       </c>
       <c r="J109">
-        <v>0.456645</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
+        <v>0.45664500000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>179755657</v>
       </c>
@@ -4504,10 +4564,10 @@
         <v>42545</v>
       </c>
       <c r="J110">
-        <v>0.4206895</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10">
+        <v>0.42068949999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>180581071</v>
       </c>
@@ -4533,10 +4593,10 @@
         <v>42545</v>
       </c>
       <c r="J111">
-        <v>0.4189303</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10">
+        <v>0.41893029999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>182220744</v>
       </c>
@@ -4565,7 +4625,7 @@
         <v>0.437875658</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2909150089</v>
       </c>
@@ -4591,10 +4651,10 @@
         <v>43490</v>
       </c>
       <c r="J113">
-        <v>0.485651433</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10">
+        <v>0.48565143300000002</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>204264503</v>
       </c>
@@ -4623,7 +4683,7 @@
         <v>0.4666788</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>46295352</v>
       </c>
@@ -4649,10 +4709,10 @@
         <v>42545</v>
       </c>
       <c r="J115">
-        <v>0.447078139</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10">
+        <v>0.44707813899999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>51679486</v>
       </c>
@@ -4678,10 +4738,10 @@
         <v>42545</v>
       </c>
       <c r="J116">
-        <v>0.41014114</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
+        <v>0.41014114000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2777648638</v>
       </c>
@@ -4710,10 +4770,10 @@
         <v>43105</v>
       </c>
       <c r="J117">
-        <v>0.6758274440000001</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
+        <v>0.67582744400000005</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>519248777</v>
       </c>
@@ -4742,10 +4802,10 @@
         <v>42545</v>
       </c>
       <c r="J118">
-        <v>0.5663113</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
+        <v>0.56631129999999996</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2779134260</v>
       </c>
@@ -4771,10 +4831,10 @@
         <v>43105</v>
       </c>
       <c r="J119">
-        <v>0.474012226</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
+        <v>0.47401222599999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2778721985</v>
       </c>
@@ -4800,10 +4860,10 @@
         <v>43105</v>
       </c>
       <c r="J120">
-        <v>0.475134015</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
+        <v>0.47513401500000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2779341262</v>
       </c>
@@ -4829,10 +4889,10 @@
         <v>43105</v>
       </c>
       <c r="J121">
-        <v>0.4824086</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10">
+        <v>0.48240860000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2779379848</v>
       </c>
@@ -4861,10 +4921,10 @@
         <v>43105</v>
       </c>
       <c r="J122">
-        <v>0.462463975</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10">
+        <v>0.46246397500000003</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2779644171</v>
       </c>
@@ -4896,7 +4956,7 @@
         <v>0.487470984</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2780356881</v>
       </c>
@@ -4922,10 +4982,10 @@
         <v>43105</v>
       </c>
       <c r="J124">
-        <v>0.5156435</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10">
+        <v>0.51564350000000003</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2781001862</v>
       </c>
@@ -4954,10 +5014,10 @@
         <v>43105</v>
       </c>
       <c r="J125">
-        <v>0.4889263</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10">
+        <v>0.48892629999999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2781009399</v>
       </c>
@@ -4983,10 +5043,10 @@
         <v>43105</v>
       </c>
       <c r="J126">
-        <v>0.5097849</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10">
+        <v>0.50978489999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2779872411</v>
       </c>
@@ -5012,10 +5072,10 @@
         <v>43105</v>
       </c>
       <c r="J127">
-        <v>0.471635371</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10">
+        <v>0.47163537100000003</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2781413609</v>
       </c>
@@ -5044,7 +5104,7 @@
         <v>0.44435975</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2776012195</v>
       </c>
@@ -5073,7 +5133,7 @@
         <v>0.5406995</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2777863537</v>
       </c>
@@ -5102,10 +5162,10 @@
         <v>43105</v>
       </c>
       <c r="J130">
-        <v>0.450505316</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10">
+        <v>0.45050531599999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2776178081</v>
       </c>
@@ -5134,10 +5194,10 @@
         <v>43105</v>
       </c>
       <c r="J131">
-        <v>0.411728173</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10">
+        <v>0.41172817299999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2777020439</v>
       </c>
@@ -5166,10 +5226,10 @@
         <v>43105</v>
       </c>
       <c r="J132">
-        <v>0.487185627</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10">
+        <v>0.48718562700000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2776178377</v>
       </c>
@@ -5198,10 +5258,10 @@
         <v>43105</v>
       </c>
       <c r="J133">
-        <v>0.480531484</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10">
+        <v>0.48053148400000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>65414064</v>
       </c>
@@ -5230,10 +5290,10 @@
         <v>42545</v>
       </c>
       <c r="J134">
-        <v>0.468291223</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10">
+        <v>0.46829122299999998</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>107130276</v>
       </c>
@@ -5262,10 +5322,10 @@
         <v>42545</v>
       </c>
       <c r="J135">
-        <v>0.454252273</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10">
+        <v>0.45425227299999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2776102371</v>
       </c>
@@ -5294,10 +5354,10 @@
         <v>43105</v>
       </c>
       <c r="J136">
-        <v>0.556363344</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10">
+        <v>0.55636334399999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>8891405</v>
       </c>
@@ -5323,10 +5383,10 @@
         <v>42545</v>
       </c>
       <c r="J137">
-        <v>0.442875534</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10">
+        <v>0.44287553400000002</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>40827391</v>
       </c>
@@ -5358,7 +5418,7 @@
         <v>0.430758268</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2777120189</v>
       </c>
@@ -5384,10 +5444,10 @@
         <v>43105</v>
       </c>
       <c r="J139">
-        <v>0.44305563</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10">
+        <v>0.44305562999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2777269905</v>
       </c>
@@ -5419,7 +5479,7 @@
         <v>0.420717746</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>27415008</v>
       </c>
@@ -5445,10 +5505,10 @@
         <v>42545</v>
       </c>
       <c r="J141">
-        <v>0.446659</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10">
+        <v>0.44665899999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>22070199</v>
       </c>
@@ -5474,10 +5534,10 @@
         <v>42545</v>
       </c>
       <c r="J142">
-        <v>0.5413762</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10">
+        <v>0.54137619999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>17022365</v>
       </c>
@@ -5503,10 +5563,10 @@
         <v>42545</v>
       </c>
       <c r="J143">
-        <v>0.440203428</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10">
+        <v>0.44020342800000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>12174686</v>
       </c>
@@ -5532,10 +5592,10 @@
         <v>42545</v>
       </c>
       <c r="J144">
-        <v>0.4574871</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10">
+        <v>0.45748709999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2777042776</v>
       </c>
@@ -5561,10 +5621,10 @@
         <v>43105</v>
       </c>
       <c r="J145">
-        <v>0.5386634</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10">
+        <v>0.53866340000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>187651312</v>
       </c>
@@ -5590,10 +5650,10 @@
         <v>42545</v>
       </c>
       <c r="J146">
-        <v>0.457288265</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10">
+        <v>0.45728826500000003</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>112964050</v>
       </c>
@@ -5622,10 +5682,10 @@
         <v>42545</v>
       </c>
       <c r="J147">
-        <v>0.4209626</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10">
+        <v>0.42096260000000002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>160735492</v>
       </c>
@@ -5654,10 +5714,10 @@
         <v>42545</v>
       </c>
       <c r="J148">
-        <v>0.486594379</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10">
+        <v>0.48659437900000002</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2908647359</v>
       </c>
@@ -5686,10 +5746,10 @@
         <v>43490</v>
       </c>
       <c r="J149">
-        <v>0.5370196</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10">
+        <v>0.53701960000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>534529494</v>
       </c>
@@ -5715,10 +5775,10 @@
         <v>42545</v>
       </c>
       <c r="J150">
-        <v>0.4446493</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10">
+        <v>0.44464930000000003</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>188084074</v>
       </c>
@@ -5747,7 +5807,7 @@
         <v>0.5308254</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>555293320</v>
       </c>
@@ -5776,10 +5836,10 @@
         <v>42545</v>
       </c>
       <c r="J152">
-        <v>0.437699765</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10">
+        <v>0.43769976500000002</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2780724011</v>
       </c>
@@ -5808,7 +5868,7 @@
         <v>0.620207548</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>116675565</v>
       </c>
@@ -5834,10 +5894,10 @@
         <v>42545</v>
       </c>
       <c r="J154">
-        <v>0.5343188</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10">
+        <v>0.53431879999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>166888038</v>
       </c>
@@ -5863,10 +5923,10 @@
         <v>42545</v>
       </c>
       <c r="J155">
-        <v>0.486139774</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10">
+        <v>0.48613977400000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2780560020</v>
       </c>
@@ -5892,10 +5952,10 @@
         <v>43105</v>
       </c>
       <c r="J156">
-        <v>0.439393461</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10">
+        <v>0.43939346099999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>159654299</v>
       </c>
@@ -5924,10 +5984,10 @@
         <v>42545</v>
       </c>
       <c r="J157">
-        <v>0.408061653</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10">
+        <v>0.40806165300000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>148834064</v>
       </c>
@@ -5956,7 +6016,7 @@
         <v>0.4449301</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2522874641</v>
       </c>
@@ -5982,10 +6042,10 @@
         <v>42643</v>
       </c>
       <c r="J159">
-        <v>0.5033383</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10">
+        <v>0.50333830000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>138816342</v>
       </c>
@@ -6014,10 +6074,10 @@
         <v>42545</v>
       </c>
       <c r="J160">
-        <v>0.5511164670000001</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10">
+        <v>0.55111646700000005</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>50522688</v>
       </c>
@@ -6043,10 +6103,10 @@
         <v>42545</v>
       </c>
       <c r="J161">
-        <v>0.412790835</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10">
+        <v>0.41279083500000002</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>159047783</v>
       </c>
@@ -6072,10 +6132,10 @@
         <v>42545</v>
       </c>
       <c r="J162">
-        <v>0.457334369</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10">
+        <v>0.45733436900000002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>149923435</v>
       </c>
@@ -6101,10 +6161,10 @@
         <v>42545</v>
       </c>
       <c r="J163">
-        <v>0.4070065</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10">
+        <v>0.40700649999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>42972112</v>
       </c>
@@ -6130,10 +6190,10 @@
         <v>42545</v>
       </c>
       <c r="J164">
-        <v>0.406581253</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10">
+        <v>0.40658125299999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>39549134</v>
       </c>
@@ -6165,7 +6225,7 @@
         <v>0.441666842</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>545542383</v>
       </c>
@@ -6194,10 +6254,10 @@
         <v>42545</v>
       </c>
       <c r="J166">
-        <v>0.408776432</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10">
+        <v>0.40877643200000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>187212893</v>
       </c>
@@ -6226,10 +6286,10 @@
         <v>42545</v>
       </c>
       <c r="J167">
-        <v>0.412734032</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10">
+        <v>0.41273403199999997</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>194828623</v>
       </c>
@@ -6258,10 +6318,10 @@
         <v>42545</v>
       </c>
       <c r="J168">
-        <v>0.441293538</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10">
+        <v>0.44129353799999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>203014093</v>
       </c>
@@ -6287,10 +6347,10 @@
         <v>42545</v>
       </c>
       <c r="J169">
-        <v>0.4235229</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10">
+        <v>0.42352289999999998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>512399662</v>
       </c>
@@ -6319,10 +6379,10 @@
         <v>42545</v>
       </c>
       <c r="J170">
-        <v>0.451956958</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10">
+        <v>0.45195695800000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>71924100</v>
       </c>
@@ -6351,7 +6411,7 @@
         <v>42545</v>
       </c>
       <c r="J171">
-        <v>0.426223546</v>
+        <v>0.42622354600000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>